<commit_message>
Power table and bringup report updated
</commit_message>
<xml_diff>
--- a/Electronics/3_Calculations&Simulations/Power Table.xlsx
+++ b/Electronics/3_Calculations&Simulations/Power Table.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Flexi-TEER\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Flexi-TEER\Electronics\3_Calculations&amp;Simulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BC026C-4066-4D75-B113-3BCC0C7D5954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
   <si>
     <t>Rail</t>
   </si>
@@ -152,12 +153,15 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>LCD backlight</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -546,11 +550,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,7 +649,7 @@
         <v>14.9</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G11" si="0">F3*E3</f>
+        <f t="shared" ref="G3:G12" si="0">F3*E3</f>
         <v>29.8</v>
       </c>
       <c r="H3" s="6" t="s">
@@ -880,25 +884,42 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F12" s="3" t="s">
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>100</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="4">
-        <f>SUM(G2:G11)</f>
-        <v>47.870000000000005</v>
-      </c>
-      <c r="H12" s="4"/>
+      <c r="G13" s="4">
+        <f>SUM(G2:G12)</f>
+        <v>147.87</v>
+      </c>
+      <c r="H13" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="link"/>
-    <hyperlink ref="D3" r:id="rId2" display="link"/>
-    <hyperlink ref="D5" r:id="rId3"/>
-    <hyperlink ref="D6" r:id="rId4"/>
-    <hyperlink ref="D9" r:id="rId5"/>
-    <hyperlink ref="D10" r:id="rId6"/>
-    <hyperlink ref="D11" r:id="rId7"/>
-    <hyperlink ref="D4" r:id="rId8" display="link"/>
+    <hyperlink ref="D2" r:id="rId1" display="link" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" display="link" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D4" r:id="rId8" display="link" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId9"/>

</xml_diff>